<commit_message>
fix: create name data file, add rounding data, the validator has been fixedÐ, add test negative value, replaced test filesÑ
</commit_message>
<xml_diff>
--- a/tests/data/abc_test.xlsx
+++ b/tests/data/abc_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WinUser\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WinUser\PycharmProjects\abc_test\pyAnalysis\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B805502-36B4-425D-AE94-30A161DFA3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0F962C-CAC7-4DC4-8514-AA3033059059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,11 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>код
- идентификатор
- PLU</t>
-  </si>
-  <si>
     <t>наименование анализируемых позиций</t>
   </si>
   <si>
@@ -46,6 +41,9 @@
   </si>
   <si>
     <t>Товар 5</t>
+  </si>
+  <si>
+    <t>код идентификатор PLU</t>
   </si>
 </sst>
 </file>
@@ -318,23 +316,26 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
     <col min="3" max="3" width="63.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -342,7 +343,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>100</v>
@@ -353,7 +354,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>50</v>
@@ -364,10 +365,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -375,7 +376,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>20</v>
@@ -386,7 +387,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -394,5 +395,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: reading files in .csv format and her tests
</commit_message>
<xml_diff>
--- a/tests/data/abc_test.xlsx
+++ b/tests/data/abc_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WinUser\PycharmProjects\abc_test\pyAnalysis\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0F962C-CAC7-4DC4-8514-AA3033059059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E0A66F-43D7-42A3-BBFB-A648F839074E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="шаблон" sheetId="1" r:id="rId1"/>

</xml_diff>